<commit_message>
Version 3 for production
</commit_message>
<xml_diff>
--- a/hardware/Version_03/BOM.xlsx
+++ b/hardware/Version_03/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritzkemper/Documents/GitHub/Phoenix/raspicam/hardware/Version_03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1CC54E-C3BD-C34A-B793-8913BE1B85BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D117FF-2377-2544-AA21-4A8A45DC92B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-39040" yWindow="3860" windowWidth="28040" windowHeight="17440" xr2:uid="{A2F641CC-4B65-0948-A438-E1537E4BAE8D}"/>
+    <workbookView xWindow="2200" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{A2F641CC-4B65-0948-A438-E1537E4BAE8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -932,13 +932,14 @@
       <c r="E27" t="s">
         <v>55</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F17" r:id="rId1" xr:uid="{33C74C6C-E30A-864B-B6EB-63B17EE0D63B}"/>
+    <hyperlink ref="F27" r:id="rId2" xr:uid="{9398C1EC-96BF-F845-A6CF-231716F43F3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>